<commit_message>
more adjustments for reports - probably done
</commit_message>
<xml_diff>
--- a/graphics_calculations.xlsx
+++ b/graphics_calculations.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="6080" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Try 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
   <si>
     <t>leftBound</t>
   </si>
@@ -146,6 +147,56 @@
   <si>
     <t>BB</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">leftBound = (int) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">(reportgrid_width - ( reportgrid_width * (0.1 * (10 - adjustedResult_X_axis ))) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(widget_width/widget_width_scale_factor)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+                    </t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -244,9 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -258,9 +306,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,6 +321,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,34 +621,34 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="B3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -609,7 +660,7 @@
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -618,14 +669,12 @@
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="8"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -638,25 +687,25 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <f xml:space="preserve"> +C7 - +G7 + +J7</f>
-        <v>217.59999999999997</v>
-      </c>
-      <c r="C7" s="6">
+        <v>197.59999999999997</v>
+      </c>
+      <c r="C7" s="5">
         <f xml:space="preserve"> +D7 - +E7</f>
         <v>225.59999999999997</v>
       </c>
       <c r="D7" s="1">
         <v>564</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f xml:space="preserve"> (+D7 * ( 0.1 * ( 10 - +F7)))</f>
         <v>338.40000000000003</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f xml:space="preserve"> (+H7 / +I7 )</f>
         <v>28</v>
       </c>
@@ -666,34 +715,32 @@
       <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="1">
-        <v>20</v>
-      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <f xml:space="preserve"> +C8 - +G8 + +J8</f>
-        <v>221.59999999999997</v>
-      </c>
-      <c r="C8" s="6">
+        <v>197.59999999999997</v>
+      </c>
+      <c r="C8" s="5">
         <f xml:space="preserve"> +D8 - +E8</f>
         <v>225.59999999999997</v>
       </c>
       <c r="D8" s="1">
         <v>564</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f xml:space="preserve"> (+D8 * ( 0.1 * ( 10 - +F8)))</f>
         <v>338.40000000000003</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f xml:space="preserve"> (+H8 / +I8 )</f>
         <v>28</v>
       </c>
@@ -703,36 +750,33 @@
       <c r="I8" s="1">
         <v>2</v>
       </c>
-      <c r="J8" s="10">
-        <f>F8 * 6</f>
-        <v>24</v>
-      </c>
+      <c r="J8" s="8"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <f xml:space="preserve"> +C9 - +G9 + +J9</f>
-        <v>197.59999999999997</v>
-      </c>
-      <c r="C9" s="6">
+        <v>173.59999999999997</v>
+      </c>
+      <c r="C9" s="5">
         <f xml:space="preserve"> +D9 - +E9</f>
         <v>201.59999999999997</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <f>564 - 60</f>
         <v>504</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f xml:space="preserve"> (+D9 * ( 0.1 * ( 10 - +F9)))</f>
         <v>302.40000000000003</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f xml:space="preserve"> (+H9 / +I9 )</f>
         <v>28</v>
       </c>
@@ -742,48 +786,45 @@
       <c r="I9" s="1">
         <v>2</v>
       </c>
-      <c r="J9" s="10">
-        <f>F9 * 6</f>
-        <v>24</v>
-      </c>
+      <c r="J9" s="8"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <f xml:space="preserve"> +C11 - +G11 + +J11</f>
-        <v>556</v>
-      </c>
-      <c r="C11" s="6">
+        <v>536</v>
+      </c>
+      <c r="C11" s="5">
         <f xml:space="preserve"> +D11 - +E11</f>
         <v>564</v>
       </c>
       <c r="D11" s="1">
         <v>564</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f xml:space="preserve"> (+D11 * ( 0.1 * ( 10 - +F11)))</f>
         <v>0</v>
       </c>
       <c r="F11" s="1">
         <v>10</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f xml:space="preserve"> (+H11 / +I11 )</f>
         <v>28</v>
       </c>
@@ -793,34 +834,32 @@
       <c r="I11" s="1">
         <v>2</v>
       </c>
-      <c r="J11" s="1">
-        <v>20</v>
-      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <f xml:space="preserve"> +C12 - +G12 + +J12</f>
-        <v>596</v>
-      </c>
-      <c r="C12" s="6">
+        <v>536</v>
+      </c>
+      <c r="C12" s="5">
         <f xml:space="preserve"> +D12 - +E12</f>
         <v>564</v>
       </c>
       <c r="D12" s="1">
         <v>564</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <f xml:space="preserve"> (+D12 * ( 0.1 * ( 10 - +F12)))</f>
         <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>10</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f xml:space="preserve"> (+H12 / +I12 )</f>
         <v>28</v>
       </c>
@@ -830,36 +869,33 @@
       <c r="I12" s="1">
         <v>2</v>
       </c>
-      <c r="J12" s="10">
-        <f>F12 * 6</f>
-        <v>60</v>
-      </c>
+      <c r="J12" s="8"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <f xml:space="preserve"> +C13 - +G13 + +J13</f>
-        <v>536</v>
-      </c>
-      <c r="C13" s="6">
+        <v>476</v>
+      </c>
+      <c r="C13" s="5">
         <f xml:space="preserve"> +D13 - +E13</f>
         <v>504</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="8">
         <f>564 - 60</f>
         <v>504</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f xml:space="preserve"> (+D13 * ( 0.1 * ( 10 - +F13)))</f>
         <v>0</v>
       </c>
       <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f xml:space="preserve"> (+H13 / +I13 )</f>
         <v>28</v>
       </c>
@@ -869,48 +905,45 @@
       <c r="I13" s="1">
         <v>2</v>
       </c>
-      <c r="J13" s="10">
-        <f>F13 * 6</f>
-        <v>60</v>
-      </c>
+      <c r="J13" s="8"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <f xml:space="preserve"> +C15 - +G15 + +J15</f>
-        <v>104.79999999999995</v>
-      </c>
-      <c r="C15" s="6">
+        <v>84.799999999999955</v>
+      </c>
+      <c r="C15" s="5">
         <f xml:space="preserve"> +D15 - +E15</f>
         <v>112.79999999999995</v>
       </c>
       <c r="D15" s="1">
         <v>564</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f xml:space="preserve"> (+D15 * ( 0.1 * ( 10 - +F15)))</f>
         <v>451.20000000000005</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f xml:space="preserve"> (+H15 / +I15 )</f>
         <v>28</v>
       </c>
@@ -920,34 +953,32 @@
       <c r="I15" s="1">
         <v>2</v>
       </c>
-      <c r="J15" s="1">
-        <v>20</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <f xml:space="preserve"> +C16 - +G16 + +J16</f>
-        <v>96.799999999999955</v>
-      </c>
-      <c r="C16" s="6">
+        <v>84.799999999999955</v>
+      </c>
+      <c r="C16" s="5">
         <f xml:space="preserve"> +D16 - +E16</f>
         <v>112.79999999999995</v>
       </c>
       <c r="D16" s="1">
         <v>564</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <f xml:space="preserve"> (+D16 * ( 0.1 * ( 10 - +F16)))</f>
         <v>451.20000000000005</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f xml:space="preserve"> (+H16 / +I16 )</f>
         <v>28</v>
       </c>
@@ -957,36 +988,33 @@
       <c r="I16" s="1">
         <v>2</v>
       </c>
-      <c r="J16" s="10">
-        <f>F16 * 6</f>
-        <v>12</v>
-      </c>
+      <c r="J16" s="8"/>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <f xml:space="preserve"> +C17 - +G17 + +J17</f>
-        <v>84.799999999999955</v>
-      </c>
-      <c r="C17" s="6">
+        <v>72.799999999999955</v>
+      </c>
+      <c r="C17" s="5">
         <f xml:space="preserve"> +D17 - +E17</f>
         <v>100.79999999999995</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="8">
         <f>564 - 60</f>
         <v>504</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <f xml:space="preserve"> (+D17 * ( 0.1 * ( 10 - +F17)))</f>
         <v>403.20000000000005</v>
       </c>
       <c r="F17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f xml:space="preserve"> (+H17 / +I17 )</f>
         <v>28</v>
       </c>
@@ -996,15 +1024,12 @@
       <c r="I17" s="1">
         <v>2</v>
       </c>
-      <c r="J17" s="10">
-        <f>F17 * 6</f>
-        <v>12</v>
-      </c>
+      <c r="J17" s="8"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="8"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1017,7 +1042,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1030,15 +1055,15 @@
     </row>
     <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1050,7 +1075,7 @@
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f xml:space="preserve"> 564 / 2</f>
         <v>282</v>
       </c>
@@ -1068,7 +1093,7 @@
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1089,7 +1114,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="8"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1104,20 +1129,20 @@
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <f>+C24 - +D24 + H24</f>
-        <v>338.40000000000003</v>
+        <v>358.40000000000003</v>
       </c>
       <c r="C24" s="1">
         <v>564</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f xml:space="preserve"> +E24 + ( +F24 / +G24 )</f>
-        <v>245.59999999999997</v>
-      </c>
-      <c r="E24" s="6">
+        <v>225.59999999999997</v>
+      </c>
+      <c r="E24" s="5">
         <f>+$B$7</f>
-        <v>217.59999999999997</v>
+        <v>197.59999999999997</v>
       </c>
       <c r="F24" s="1">
         <v>56</v>
@@ -1134,20 +1159,20 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <f>+C25 - +D25 + H25</f>
-        <v>438.40000000000003</v>
+        <v>458.40000000000003</v>
       </c>
       <c r="C25" s="1">
         <v>564</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <f xml:space="preserve"> +E25 + ( +F25 / +G25 )</f>
-        <v>245.59999999999997</v>
-      </c>
-      <c r="E25" s="6">
+        <v>225.59999999999997</v>
+      </c>
+      <c r="E25" s="5">
         <f>+$B$7</f>
-        <v>217.59999999999997</v>
+        <v>197.59999999999997</v>
       </c>
       <c r="F25" s="1">
         <v>56</v>
@@ -1155,7 +1180,7 @@
       <c r="G25" s="1">
         <v>2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="9">
         <f>(10 - F7) * 20</f>
         <v>120</v>
       </c>
@@ -1165,20 +1190,20 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <f>+C26 - +D26 + H26</f>
-        <v>284.40000000000003</v>
-      </c>
-      <c r="C26" s="10">
+        <v>304.40000000000003</v>
+      </c>
+      <c r="C26" s="8">
         <v>510</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <f xml:space="preserve"> +E26 + ( +F26 / +G26 )</f>
-        <v>245.59999999999997</v>
-      </c>
-      <c r="E26" s="6">
+        <v>225.59999999999997</v>
+      </c>
+      <c r="E26" s="5">
         <f>+$B$7</f>
-        <v>217.59999999999997</v>
+        <v>197.59999999999997</v>
       </c>
       <c r="F26" s="1">
         <v>56</v>
@@ -1197,20 +1222,20 @@
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="7">
         <f>(+C27 - +D27 )+ H27</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1">
         <v>564</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <f xml:space="preserve"> +E27 + ( +F27 / +G27 )</f>
-        <v>584</v>
-      </c>
-      <c r="E27" s="6">
+        <v>564</v>
+      </c>
+      <c r="E27" s="5">
         <f>+$B$11</f>
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="F27" s="1">
         <v>56</v>
@@ -1227,20 +1252,20 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="9">
+      <c r="B28" s="7">
         <f t="shared" ref="B28:B29" si="0">(+C28 - +D28 )+ H28</f>
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <v>564</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <f t="shared" ref="D28:D29" si="1" xml:space="preserve"> +E28 + ( +F28 / +G28 )</f>
-        <v>624</v>
-      </c>
-      <c r="E28" s="9">
+        <v>564</v>
+      </c>
+      <c r="E28" s="7">
         <f>+$B$12</f>
-        <v>596</v>
+        <v>536</v>
       </c>
       <c r="F28" s="1">
         <v>56</v>
@@ -1248,7 +1273,7 @@
       <c r="G28" s="1">
         <v>2</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="9">
         <f>(10 - F11) * 20</f>
         <v>0</v>
       </c>
@@ -1258,20 +1283,20 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="9">
+      <c r="B29" s="7">
         <f t="shared" si="0"/>
-        <v>-54</v>
-      </c>
-      <c r="C29" s="10">
+        <v>-34</v>
+      </c>
+      <c r="C29" s="8">
         <v>510</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <f t="shared" si="1"/>
-        <v>584</v>
-      </c>
-      <c r="E29" s="6">
+        <v>564</v>
+      </c>
+      <c r="E29" s="5">
         <f>+$B$11</f>
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="F29" s="1">
         <v>56</v>
@@ -1288,7 +1313,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="8"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1303,20 +1328,20 @@
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="7">
         <f>+C31 - +D31 + H31</f>
-        <v>471.20000000000005</v>
+        <v>483.20000000000005</v>
       </c>
       <c r="C31" s="1">
         <v>564</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <f xml:space="preserve"> +E31 + ( +F31 / +G31 )</f>
-        <v>112.79999999999995</v>
-      </c>
-      <c r="E31" s="9">
+        <v>100.79999999999995</v>
+      </c>
+      <c r="E31" s="7">
         <f>+$B$17</f>
-        <v>84.799999999999955</v>
+        <v>72.799999999999955</v>
       </c>
       <c r="F31" s="1">
         <v>56</v>
@@ -1333,20 +1358,20 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="9">
+      <c r="B32" s="7">
         <f>+C32 - +D32 + H32</f>
-        <v>611.20000000000005</v>
+        <v>623.20000000000005</v>
       </c>
       <c r="C32" s="1">
         <v>564</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <f xml:space="preserve"> +E32 + ( +F32 / +G32 )</f>
-        <v>112.79999999999995</v>
-      </c>
-      <c r="E32" s="9">
+        <v>100.79999999999995</v>
+      </c>
+      <c r="E32" s="7">
         <f t="shared" ref="E32:E33" si="2">+$B$17</f>
-        <v>84.799999999999955</v>
+        <v>72.799999999999955</v>
       </c>
       <c r="F32" s="1">
         <v>56</v>
@@ -1354,7 +1379,7 @@
       <c r="G32" s="1">
         <v>2</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="9">
         <f>(10 - F17) * 20</f>
         <v>160</v>
       </c>
@@ -1364,20 +1389,20 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <f>+C33 - +D33 + H33</f>
-        <v>557.20000000000005</v>
-      </c>
-      <c r="C33" s="10">
+        <v>569.20000000000005</v>
+      </c>
+      <c r="C33" s="8">
         <v>510</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <f xml:space="preserve"> +E33 + ( +F33 / +G33 )</f>
-        <v>112.79999999999995</v>
-      </c>
-      <c r="E33" s="9">
+        <v>100.79999999999995</v>
+      </c>
+      <c r="E33" s="7">
         <f t="shared" si="2"/>
-        <v>84.799999999999955</v>
+        <v>72.799999999999955</v>
       </c>
       <c r="F33" s="1">
         <v>56</v>
@@ -1385,7 +1410,7 @@
       <c r="G33" s="1">
         <v>2</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="9">
         <f>(10 - F17) * 20</f>
         <v>160</v>
       </c>
@@ -1395,7 +1420,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="8"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1408,7 +1433,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="8"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1421,7 +1446,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="8"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1434,7 +1459,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="8"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1447,7 +1472,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="8"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1460,7 +1485,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="8"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1473,7 +1498,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
-      <c r="B40" s="8"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1486,7 +1511,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="8"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1569,4 +1594,1023 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:T46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="11" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <f xml:space="preserve"> +C7 - +G7 + +J7</f>
+        <v>217.59999999999997</v>
+      </c>
+      <c r="C7" s="5">
+        <f xml:space="preserve"> +D7 - +E7</f>
+        <v>225.59999999999997</v>
+      </c>
+      <c r="D7" s="1">
+        <v>564</v>
+      </c>
+      <c r="E7" s="5">
+        <f xml:space="preserve"> (+D7 * ( 0.1 * ( 10 - +F7)))</f>
+        <v>338.40000000000003</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <f xml:space="preserve"> (+H7 / +I7 )</f>
+        <v>28</v>
+      </c>
+      <c r="H7" s="1">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7">
+        <f xml:space="preserve"> +C8 - +G8 + +J8</f>
+        <v>221.59999999999997</v>
+      </c>
+      <c r="C8" s="5">
+        <f xml:space="preserve"> +D8 - +E8</f>
+        <v>225.59999999999997</v>
+      </c>
+      <c r="D8" s="1">
+        <v>564</v>
+      </c>
+      <c r="E8" s="5">
+        <f xml:space="preserve"> (+D8 * ( 0.1 * ( 10 - +F8)))</f>
+        <v>338.40000000000003</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
+        <f xml:space="preserve"> (+H8 / +I8 )</f>
+        <v>28</v>
+      </c>
+      <c r="H8" s="1">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="8">
+        <f>F8 * 6</f>
+        <v>24</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <f xml:space="preserve"> +C9 - +G9 + +J9</f>
+        <v>197.59999999999997</v>
+      </c>
+      <c r="C9" s="5">
+        <f xml:space="preserve"> +D9 - +E9</f>
+        <v>201.59999999999997</v>
+      </c>
+      <c r="D9" s="8">
+        <f>564 - 60</f>
+        <v>504</v>
+      </c>
+      <c r="E9" s="5">
+        <f xml:space="preserve"> (+D9 * ( 0.1 * ( 10 - +F9)))</f>
+        <v>302.40000000000003</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <f xml:space="preserve"> (+H9 / +I9 )</f>
+        <v>28</v>
+      </c>
+      <c r="H9" s="1">
+        <v>56</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="8">
+        <f>F9 * 6</f>
+        <v>24</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7">
+        <f xml:space="preserve"> +C11 - +G11 + +J11</f>
+        <v>556</v>
+      </c>
+      <c r="C11" s="5">
+        <f xml:space="preserve"> +D11 - +E11</f>
+        <v>564</v>
+      </c>
+      <c r="D11" s="1">
+        <v>564</v>
+      </c>
+      <c r="E11" s="5">
+        <f xml:space="preserve"> (+D11 * ( 0.1 * ( 10 - +F11)))</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <f xml:space="preserve"> (+H11 / +I11 )</f>
+        <v>28</v>
+      </c>
+      <c r="H11" s="1">
+        <v>56</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <f xml:space="preserve"> +C12 - +G12 + +J12</f>
+        <v>596</v>
+      </c>
+      <c r="C12" s="5">
+        <f xml:space="preserve"> +D12 - +E12</f>
+        <v>564</v>
+      </c>
+      <c r="D12" s="1">
+        <v>564</v>
+      </c>
+      <c r="E12" s="5">
+        <f xml:space="preserve"> (+D12 * ( 0.1 * ( 10 - +F12)))</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5">
+        <f xml:space="preserve"> (+H12 / +I12 )</f>
+        <v>28</v>
+      </c>
+      <c r="H12" s="1">
+        <v>56</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="8">
+        <f>F12 * 6</f>
+        <v>60</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <f xml:space="preserve"> +C13 - +G13 + +J13</f>
+        <v>536</v>
+      </c>
+      <c r="C13" s="5">
+        <f xml:space="preserve"> +D13 - +E13</f>
+        <v>504</v>
+      </c>
+      <c r="D13" s="8">
+        <f>564 - 60</f>
+        <v>504</v>
+      </c>
+      <c r="E13" s="5">
+        <f xml:space="preserve"> (+D13 * ( 0.1 * ( 10 - +F13)))</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5">
+        <f xml:space="preserve"> (+H13 / +I13 )</f>
+        <v>28</v>
+      </c>
+      <c r="H13" s="1">
+        <v>56</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8">
+        <f>F13 * 6</f>
+        <v>60</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7">
+        <f xml:space="preserve"> +C15 - +G15 + +J15</f>
+        <v>104.79999999999995</v>
+      </c>
+      <c r="C15" s="5">
+        <f xml:space="preserve"> +D15 - +E15</f>
+        <v>112.79999999999995</v>
+      </c>
+      <c r="D15" s="1">
+        <v>564</v>
+      </c>
+      <c r="E15" s="5">
+        <f xml:space="preserve"> (+D15 * ( 0.1 * ( 10 - +F15)))</f>
+        <v>451.20000000000005</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <f xml:space="preserve"> (+H15 / +I15 )</f>
+        <v>28</v>
+      </c>
+      <c r="H15" s="1">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7">
+        <f xml:space="preserve"> +C16 - +G16 + +J16</f>
+        <v>96.799999999999955</v>
+      </c>
+      <c r="C16" s="5">
+        <f xml:space="preserve"> +D16 - +E16</f>
+        <v>112.79999999999995</v>
+      </c>
+      <c r="D16" s="1">
+        <v>564</v>
+      </c>
+      <c r="E16" s="5">
+        <f xml:space="preserve"> (+D16 * ( 0.1 * ( 10 - +F16)))</f>
+        <v>451.20000000000005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5">
+        <f xml:space="preserve"> (+H16 / +I16 )</f>
+        <v>28</v>
+      </c>
+      <c r="H16" s="1">
+        <v>56</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" s="8">
+        <f>F16 * 6</f>
+        <v>12</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <f xml:space="preserve"> +C17 - +G17 + +J17</f>
+        <v>84.799999999999955</v>
+      </c>
+      <c r="C17" s="5">
+        <f xml:space="preserve"> +D17 - +E17</f>
+        <v>100.79999999999995</v>
+      </c>
+      <c r="D17" s="8">
+        <f>564 - 60</f>
+        <v>504</v>
+      </c>
+      <c r="E17" s="5">
+        <f xml:space="preserve"> (+D17 * ( 0.1 * ( 10 - +F17)))</f>
+        <v>403.20000000000005</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="5">
+        <f xml:space="preserve"> (+H17 / +I17 )</f>
+        <v>28</v>
+      </c>
+      <c r="H17" s="1">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8">
+        <f>F17 * 6</f>
+        <v>12</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="2">
+        <f xml:space="preserve"> 564 / 2</f>
+        <v>282</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7">
+        <f>+C24 - +D24 + H24</f>
+        <v>338.40000000000003</v>
+      </c>
+      <c r="C24" s="1">
+        <v>564</v>
+      </c>
+      <c r="D24" s="5">
+        <f xml:space="preserve"> +E24 + ( +F24 / +G24 )</f>
+        <v>245.59999999999997</v>
+      </c>
+      <c r="E24" s="5">
+        <f>+$B$7</f>
+        <v>217.59999999999997</v>
+      </c>
+      <c r="F24" s="1">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7">
+        <f>+C25 - +D25 + H25</f>
+        <v>438.40000000000003</v>
+      </c>
+      <c r="C25" s="1">
+        <v>564</v>
+      </c>
+      <c r="D25" s="5">
+        <f xml:space="preserve"> +E25 + ( +F25 / +G25 )</f>
+        <v>245.59999999999997</v>
+      </c>
+      <c r="E25" s="5">
+        <f>+$B$7</f>
+        <v>217.59999999999997</v>
+      </c>
+      <c r="F25" s="1">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="9">
+        <f>(10 - F7) * 20</f>
+        <v>120</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="7">
+        <f>+C26 - +D26 + H26</f>
+        <v>284.40000000000003</v>
+      </c>
+      <c r="C26" s="8">
+        <v>510</v>
+      </c>
+      <c r="D26" s="5">
+        <f xml:space="preserve"> +E26 + ( +F26 / +G26 )</f>
+        <v>245.59999999999997</v>
+      </c>
+      <c r="E26" s="5">
+        <f>+$B$7</f>
+        <v>217.59999999999997</v>
+      </c>
+      <c r="F26" s="1">
+        <v>56</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="7">
+        <f>(+C27 - +D27 )+ H27</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>564</v>
+      </c>
+      <c r="D27" s="5">
+        <f xml:space="preserve"> +E27 + ( +F27 / +G27 )</f>
+        <v>584</v>
+      </c>
+      <c r="E27" s="5">
+        <f>+$B$11</f>
+        <v>556</v>
+      </c>
+      <c r="F27" s="1">
+        <v>56</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>20</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="7">
+        <f t="shared" ref="B28:B29" si="0">(+C28 - +D28 )+ H28</f>
+        <v>-60</v>
+      </c>
+      <c r="C28" s="1">
+        <v>564</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" ref="D28:D29" si="1" xml:space="preserve"> +E28 + ( +F28 / +G28 )</f>
+        <v>624</v>
+      </c>
+      <c r="E28" s="7">
+        <f>+$B$12</f>
+        <v>596</v>
+      </c>
+      <c r="F28" s="1">
+        <v>56</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="9">
+        <f>(10 - F11) * 20</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="7">
+        <f t="shared" si="0"/>
+        <v>-54</v>
+      </c>
+      <c r="C29" s="8">
+        <v>510</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="1"/>
+        <v>584</v>
+      </c>
+      <c r="E29" s="5">
+        <f>+$B$11</f>
+        <v>556</v>
+      </c>
+      <c r="F29" s="1">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="7">
+        <f>+C31 - +D31 + H31</f>
+        <v>471.20000000000005</v>
+      </c>
+      <c r="C31" s="1">
+        <v>564</v>
+      </c>
+      <c r="D31" s="5">
+        <f xml:space="preserve"> +E31 + ( +F31 / +G31 )</f>
+        <v>112.79999999999995</v>
+      </c>
+      <c r="E31" s="7">
+        <f>+$B$17</f>
+        <v>84.799999999999955</v>
+      </c>
+      <c r="F31" s="1">
+        <v>56</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1">
+        <v>20</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7">
+        <f>+C32 - +D32 + H32</f>
+        <v>611.20000000000005</v>
+      </c>
+      <c r="C32" s="1">
+        <v>564</v>
+      </c>
+      <c r="D32" s="5">
+        <f xml:space="preserve"> +E32 + ( +F32 / +G32 )</f>
+        <v>112.79999999999995</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" ref="E32:E33" si="2">+$B$17</f>
+        <v>84.799999999999955</v>
+      </c>
+      <c r="F32" s="1">
+        <v>56</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2</v>
+      </c>
+      <c r="H32" s="9">
+        <f>(10 - F17) * 20</f>
+        <v>160</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="7">
+        <f>+C33 - +D33 + H33</f>
+        <v>557.20000000000005</v>
+      </c>
+      <c r="C33" s="8">
+        <v>510</v>
+      </c>
+      <c r="D33" s="5">
+        <f xml:space="preserve"> +E33 + ( +F33 / +G33 )</f>
+        <v>112.79999999999995</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="2"/>
+        <v>84.799999999999955</v>
+      </c>
+      <c r="F33" s="1">
+        <v>56</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2</v>
+      </c>
+      <c r="H33" s="9">
+        <f>(10 - F17) * 20</f>
+        <v>160</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:T3"/>
+    <mergeCell ref="B20:H20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>